<commit_message>
Change to Da Vinci Template. Fix Observation Resource examples Point member-match operation to build.fhir.org HREX
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-device.xlsx
+++ b/output/StructureDefinition-pdex-device.xlsx
@@ -3633,7 +3633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>173</v>
       </c>
@@ -3643,13 +3643,13 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>46</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>47</v>
@@ -7585,7 +7585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" hidden="true">
+    <row r="60">
       <c r="A60" t="s" s="2">
         <v>288</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>46</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
v1.0.0 -rev(q) add ignoreWarnings.txt message for jira.xml tooling issue
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-device.xlsx
+++ b/output/StructureDefinition-pdex-device.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="330">
   <si>
     <t>Path</t>
   </si>
@@ -588,10 +588,7 @@
     <t>This element is labeled as a modifier because the status contains the codes inactive and entered-in-error that mark the device (record)as not currently valid.</t>
   </si>
   <si>
-    <t>The availability status of the device.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/device-status|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/device-status</t>
   </si>
   <si>
     <t>.statusCode</t>
@@ -2557,7 +2554,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>115</v>
       </c>
@@ -2573,7 +2570,7 @@
         <v>46</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>39</v>
@@ -2989,7 +2986,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>134</v>
       </c>
@@ -3005,7 +3002,7 @@
         <v>46</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>39</v>
@@ -3309,7 +3306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>152</v>
       </c>
@@ -3325,7 +3322,7 @@
         <v>46</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>39</v>
@@ -3417,7 +3414,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>159</v>
       </c>
@@ -3433,7 +3430,7 @@
         <v>46</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>39</v>
@@ -3643,7 +3640,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>46</v>
@@ -3695,11 +3692,9 @@
       <c r="W23" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="X23" t="s" s="2">
+      <c r="X23" s="2"/>
+      <c r="Y23" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>39</v>
@@ -3732,10 +3727,10 @@
         <v>58</v>
       </c>
       <c r="AJ23" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AK23" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="AK23" t="s" s="2">
-        <v>180</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>39</v>
@@ -3743,7 +3738,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3766,13 +3761,13 @@
         <v>39</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>183</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>184</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3799,14 +3794,14 @@
         <v>39</v>
       </c>
       <c r="W24" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="X24" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="X24" t="s" s="2">
+      <c r="Y24" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>187</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>39</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3841,19 +3836,19 @@
         <v>39</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -3863,7 +3858,7 @@
         <v>46</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>39</v>
@@ -3875,13 +3870,13 @@
         <v>48</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3931,7 +3926,7 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -3946,18 +3941,18 @@
         <v>58</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>139</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3983,10 +3978,10 @@
         <v>48</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4037,7 +4032,7 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -4052,7 +4047,7 @@
         <v>58</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>139</v>
@@ -4063,7 +4058,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4086,13 +4081,13 @@
         <v>39</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>201</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4143,7 +4138,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -4158,18 +4153,18 @@
         <v>58</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>139</v>
       </c>
       <c r="AL27" t="s" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
         <v>204</v>
-      </c>
-    </row>
-    <row r="28" hidden="true">
-      <c r="A28" t="s" s="2">
-        <v>205</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4183,7 +4178,7 @@
         <v>46</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>39</v>
@@ -4192,13 +4187,13 @@
         <v>39</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4249,7 +4244,7 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4264,18 +4259,18 @@
         <v>58</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>139</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
         <v>209</v>
-      </c>
-    </row>
-    <row r="29" hidden="true">
-      <c r="A29" t="s" s="2">
-        <v>210</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4289,7 +4284,7 @@
         <v>46</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>39</v>
@@ -4301,10 +4296,10 @@
         <v>48</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4355,7 +4350,7 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4370,18 +4365,18 @@
         <v>58</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>139</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4395,7 +4390,7 @@
         <v>46</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>39</v>
@@ -4407,13 +4402,13 @@
         <v>48</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4463,7 +4458,7 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4478,7 +4473,7 @@
         <v>58</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>139</v>
@@ -4489,7 +4484,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4515,10 +4510,10 @@
         <v>116</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4569,7 +4564,7 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4595,7 +4590,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4701,7 +4696,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4809,7 +4804,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4919,11 +4914,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -4945,10 +4940,10 @@
         <v>48</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -4999,7 +4994,7 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>46</v>
@@ -5025,7 +5020,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5051,10 +5046,10 @@
         <v>66</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5084,11 +5079,11 @@
         <v>169</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="Y36" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>232</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>39</v>
       </c>
@@ -5105,7 +5100,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>46</v>
@@ -5120,7 +5115,7 @@
         <v>58</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>139</v>
@@ -5131,7 +5126,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5157,10 +5152,10 @@
         <v>48</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5211,7 +5206,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5226,7 +5221,7 @@
         <v>58</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>139</v>
@@ -5237,7 +5232,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5263,13 +5258,13 @@
         <v>48</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="L38" t="s" s="2">
-        <v>240</v>
-      </c>
       <c r="M38" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5319,7 +5314,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5334,7 +5329,7 @@
         <v>58</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>139</v>
@@ -5343,9 +5338,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5359,7 +5354,7 @@
         <v>46</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>39</v>
@@ -5368,13 +5363,13 @@
         <v>39</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>243</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5401,11 +5396,11 @@
         <v>39</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X39" s="2"/>
       <c r="Y39" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>39</v>
@@ -5423,7 +5418,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5449,7 +5444,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5475,10 +5470,10 @@
         <v>116</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>247</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5529,7 +5524,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5555,7 +5550,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5661,7 +5656,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5769,7 +5764,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5879,11 +5874,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -5902,13 +5897,13 @@
         <v>39</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5959,7 +5954,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>46</v>
@@ -5985,7 +5980,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6011,10 +6006,10 @@
         <v>48</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6065,7 +6060,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6091,7 +6086,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6117,10 +6112,10 @@
         <v>116</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6171,7 +6166,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6197,7 +6192,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6303,7 +6298,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6411,7 +6406,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6521,11 +6516,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6544,13 +6539,13 @@
         <v>39</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6601,7 +6596,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6627,7 +6622,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6653,10 +6648,10 @@
         <v>104</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6707,7 +6702,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -6733,7 +6728,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6759,10 +6754,10 @@
         <v>48</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6813,7 +6808,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>46</v>
@@ -6839,7 +6834,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -6865,10 +6860,10 @@
         <v>116</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -6919,7 +6914,7 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -6945,7 +6940,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7051,7 +7046,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7159,7 +7154,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7269,7 +7264,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7292,13 +7287,13 @@
         <v>39</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>280</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7349,7 +7344,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>46</v>
@@ -7375,7 +7370,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7398,13 +7393,13 @@
         <v>39</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="K58" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="K58" t="s" s="2">
+      <c r="L58" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7455,7 +7450,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7481,7 +7476,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7504,13 +7499,13 @@
         <v>39</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>287</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7561,7 +7556,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7587,7 +7582,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7610,17 +7605,17 @@
         <v>39</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>39</v>
@@ -7669,7 +7664,7 @@
         <v>39</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
@@ -7684,10 +7679,10 @@
         <v>58</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AK60" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>39</v>
@@ -7695,7 +7690,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -7718,13 +7713,13 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -7775,7 +7770,7 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -7790,10 +7785,10 @@
         <v>58</v>
       </c>
       <c r="AJ61" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AK61" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>39</v>
@@ -7801,7 +7796,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -7824,16 +7819,16 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -7883,7 +7878,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -7898,10 +7893,10 @@
         <v>58</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>39</v>
@@ -7909,7 +7904,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -7932,17 +7927,17 @@
         <v>39</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>39</v>
@@ -7991,7 +7986,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8006,10 +8001,10 @@
         <v>58</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AK63" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>39</v>
@@ -8017,7 +8012,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8043,13 +8038,13 @@
         <v>60</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8099,7 +8094,7 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8114,10 +8109,10 @@
         <v>58</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>39</v>
@@ -8125,7 +8120,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8148,13 +8143,13 @@
         <v>39</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8205,7 +8200,7 @@
         <v>39</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8220,7 +8215,7 @@
         <v>58</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>39</v>
@@ -8231,7 +8226,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8254,13 +8249,13 @@
         <v>47</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>325</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8311,7 +8306,7 @@
         <v>39</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8337,7 +8332,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8360,13 +8355,13 @@
         <v>39</v>
       </c>
       <c r="J67" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="K67" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="K67" t="s" s="2">
+      <c r="L67" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8417,7 +8412,7 @@
         <v>39</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>40</v>

</xml_diff>